<commit_message>
general table: WERs for all subsets template
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\docs\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0748B6E8-49A9-4746-BF17-425EB5D7A1CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B368F161-77EE-4063-B05E-8D04F447ADC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -241,6 +241,18 @@
   </si>
   <si>
     <t>in samples</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>clean</t>
+  </si>
+  <si>
+    <t>other</t>
   </si>
 </sst>
 </file>
@@ -250,11 +262,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -464,26 +483,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -495,10 +517,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -507,8 +529,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -522,13 +544,15 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -756,15 +780,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
@@ -773,95 +797,124 @@
         <v>9</v>
       </c>
       <c r="D1" s="15"/>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C3" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="37" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E3" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>51</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="F4" s="4">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F5" s="1">
         <v>7.1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="1">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>52</v>
       </c>
       <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F7" s="1">
         <v>6.8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="5">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -887,13 +940,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="38" t="s">
         <v>29</v>
       </c>
     </row>
@@ -952,22 +1005,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="31" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="33"/>
     </row>
     <row r="3" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -1038,7 +1091,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1053,31 +1106,31 @@
       <c r="B1" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="28"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>5</v>
       </c>
       <c r="B3" s="12">
@@ -1089,12 +1142,12 @@
       <c r="D3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>7.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="10">
         <v>150</v>
       </c>
@@ -1109,7 +1162,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="10">
         <v>200</v>
       </c>
@@ -1124,7 +1177,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="10">
         <v>250</v>
       </c>
@@ -1142,7 +1195,7 @@
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="18">
         <v>150</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -1159,7 +1212,7 @@
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="18"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="10" t="s">
         <v>46</v>
       </c>
@@ -1196,16 +1249,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1393,13 +1446,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="34" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="36" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1434,7 +1487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
tables: WERs for all subsets template
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\docs\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B368F161-77EE-4063-B05E-8D04F447ADC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D029B515-9CDC-4DBA-B735-594BE6B49AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -126,9 +126,6 @@
     <t>32k</t>
   </si>
   <si>
-    <t>dev-other</t>
-  </si>
-  <si>
     <t>FE</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Filterbanks</t>
   </si>
   <si>
-    <t>\#Temp. Integr.</t>
-  </si>
-  <si>
     <t>Kernels</t>
   </si>
   <si>
@@ -253,6 +247,12 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>Integr.</t>
+  </si>
+  <si>
+    <t>\#Temp.</t>
   </si>
 </sst>
 </file>
@@ -334,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -358,19 +358,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -405,6 +392,17 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -479,11 +477,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -496,9 +525,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -508,32 +537,23 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,18 +561,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -782,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,56 +857,59 @@
       <c r="C2" s="15"/>
       <c r="D2" s="15"/>
       <c r="E2" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="17"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="F3" s="42" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="H3" s="42" t="s">
-        <v>71</v>
+      <c r="G3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
+      <c r="E4" s="1"/>
       <c r="F4" s="4">
         <v>6.9</v>
       </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -870,16 +920,19 @@
       <c r="D5" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>7.1</v>
       </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>22</v>
@@ -887,13 +940,16 @@
       <c r="D6" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>7.1</v>
       </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
@@ -904,9 +960,12 @@
       <c r="D7" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>6.8</v>
       </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -922,70 +981,106 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A21A4E4-2D2F-46DE-B6F5-275971AEE32B}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="C4" sqref="C4:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16"/>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="39" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C4" s="1">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>6.9</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
         <v>7.1</v>
       </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+  <mergeCells count="4">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -993,10 +1088,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A2FF86-780C-455F-9277-DC3386C71D46}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1004,83 +1099,121 @@
     <col min="3" max="3" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="32" t="s">
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="33"/>
-    </row>
-    <row r="3" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3">
+      <c r="F2" s="17"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>64</v>
+      </c>
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D4" s="1">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
         <v>128</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D5" s="1">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
         <v>160</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>10</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D6" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
         <v>256</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>16</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D7" s="1">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
         <v>400</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>25</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D8" s="1">
         <v>7.3</v>
       </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C2"/>
+  <mergeCells count="4">
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A1:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C363DB-E141-4F3D-B7AC-39434B0B3278}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1099,136 +1232,186 @@
     <col min="5" max="5" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="38"/>
       <c r="E1" s="20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="25" t="s">
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="23"/>
+      <c r="B3" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="28" t="s">
+      <c r="C3" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="29"/>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="23">
+      <c r="D3" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="21">
         <v>5</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B4" s="12">
         <v>100</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22">
+        <v>7.1</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="21"/>
+      <c r="B5" s="10">
+        <v>150</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="B6" s="10">
+        <v>200</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11">
+        <v>7.1</v>
+      </c>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="19"/>
+      <c r="B7" s="10">
+        <v>250</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="24">
+      <c r="D7" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
+        <v>6</v>
+      </c>
+      <c r="B8" s="18">
+        <v>150</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11">
+        <v>7.3</v>
+      </c>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="10">
+        <v>7</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="10">
-        <v>150</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="11">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="23"/>
-      <c r="B5" s="10">
-        <v>200</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="11">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19"/>
-      <c r="B6" s="10">
-        <v>250</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="11">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10">
-        <v>6</v>
-      </c>
-      <c r="B7" s="18">
-        <v>150</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="11">
-        <v>7.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="10">
-        <v>7</v>
-      </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="11">
-        <v>7.1</v>
-      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A6"/>
+  <mergeCells count="6">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C1:D2"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1236,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="G15" sqref="D4:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1248,107 +1431,120 @@
     <col min="4" max="4" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <v>512</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="5">
-        <v>6.8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>256</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="5">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="17"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="42"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
+      <c r="D3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>128</v>
+        <v>512</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5">
+        <v>6.8</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="5">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+      <c r="E5" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>512</v>
+        <v>128</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="5">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="5">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5">
         <v>7.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>512</v>
@@ -1356,13 +1552,15 @@
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9">
         <v>64</v>
@@ -1370,115 +1568,209 @@
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="5">
-        <v>7.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E9" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
         <v>512</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="5">
-        <v>6.9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+      <c r="E10" s="5">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
         <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="5">
-        <v>7.4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>512</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="5">
-        <v>7.1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+      <c r="E12" s="5">
+        <v>6.9</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="5">
+        <v>7.4</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>512</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="5">
+        <v>7.1</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>64</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E15" s="4">
         <v>7.6</v>
       </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A375FB06-3221-44DD-B2E3-EEAFC4F977A3}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C4" sqref="C4:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" s="28"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="46"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" s="34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="C4" s="1"/>
+      <c r="D4" s="5">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C5" s="1"/>
+      <c r="D5" s="5">
         <v>6.8</v>
       </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1498,31 +1790,31 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
@@ -1530,15 +1822,15 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tables: WER in percentage, update captions
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\docs\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D029B515-9CDC-4DBA-B735-594BE6B49AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E190E4-215C-4FA7-BFC6-F402C3143E7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Feature Extractor</t>
   </si>
   <si>
-    <t>WER</t>
-  </si>
-  <si>
     <t>Gammatone</t>
   </si>
   <si>
@@ -204,18 +201,9 @@
     <t>scf_size</t>
   </si>
   <si>
-    <t>Comparison of different sizes for the layer directly on the waveform in the learnable \acrfull{SC} feature extraction.</t>
-  </si>
-  <si>
-    <t>Comparison of different feature extraction methods for a CTC model on Librispeech.</t>
-  </si>
-  <si>
     <t>Effect of pre-training the wav2vec 2.0 feature extractor using the unsupervised loss on the same data (Librispeech 960h).</t>
   </si>
   <si>
-    <t>Comparison of different inner dimensions for learnable \acrfull{SC} feature extraction.</t>
-  </si>
-  <si>
     <t>Studying the effect of the wav2vec 2.0 feature extractor's width and depth.</t>
   </si>
   <si>
@@ -253,6 +241,18 @@
   </si>
   <si>
     <t>\#Temp.</t>
+  </si>
+  <si>
+    <t>WER [\%]</t>
+  </si>
+  <si>
+    <t>Comparison of different feature extraction methods for a CTC model on LibriSpeech.</t>
+  </si>
+  <si>
+    <t>Comparison of different sizes for the layer which operates directly on the waveform in the learnable \acrfull{SC} feature extraction.</t>
+  </si>
+  <si>
+    <t>Comparison of different numbers of filters for the learnable \acrfull{SC} feature extraction.</t>
   </si>
 </sst>
 </file>
@@ -512,7 +512,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -528,13 +528,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -543,31 +558,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,26 +573,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -830,115 +821,115 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="E1" sqref="E1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="32"/>
+      <c r="E1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="17"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="A3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="34" t="s">
-        <v>69</v>
+      <c r="D3" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="4">
-        <v>6.9</v>
+      <c r="F4" s="1">
+        <v>7.1</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <v>7.1</v>
+      <c r="F5" s="4">
+        <v>6.9</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
@@ -949,16 +940,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
@@ -984,61 +975,61 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F6"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="17"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>69</v>
+      <c r="C3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1">
@@ -1049,10 +1040,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1">
@@ -1063,10 +1054,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1">
@@ -1090,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A2FF86-780C-455F-9277-DC3386C71D46}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1100,47 +1091,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
+      <c r="A1" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="17"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="E3" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>69</v>
+      <c r="F3" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1224,7 +1215,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1234,94 +1225,94 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+        <v>67</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="37"/>
+      <c r="E1" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
+      <c r="H1" s="40"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="38"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="40" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="H2" s="20"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="23"/>
-      <c r="B3" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="26" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" s="47" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>69</v>
+      <c r="D3" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>64</v>
+      </c>
+      <c r="H3" s="29" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="A4" s="35">
         <v>5</v>
       </c>
       <c r="B4" s="12">
         <v>100</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22">
+        <v>36</v>
+      </c>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15">
         <v>7.1</v>
       </c>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="21"/>
+      <c r="A5" s="35"/>
       <c r="B5" s="10">
         <v>150</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11">
@@ -1331,15 +1322,15 @@
       <c r="H5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="21"/>
+      <c r="A6" s="35"/>
       <c r="B6" s="10">
         <v>200</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" s="11"/>
       <c r="F6" s="11">
@@ -1349,15 +1340,15 @@
       <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="19"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="10">
         <v>250</v>
       </c>
       <c r="C7" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="E7" s="11"/>
       <c r="F7" s="11">
@@ -1370,14 +1361,14 @@
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="33">
         <v>150</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="11">
@@ -1390,12 +1381,12 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="11">
@@ -1422,7 +1413,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="D4:G15"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1433,49 +1424,49 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+        <v>7</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="41"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="17"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="30"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="42"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
-      <c r="D3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>69</v>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
@@ -1486,7 +1477,7 @@
         <v>512</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" s="5">
         <v>6.8</v>
@@ -1502,7 +1493,7 @@
         <v>256</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5">
         <v>7.1</v>
@@ -1518,7 +1509,7 @@
         <v>128</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="5">
         <v>7.2</v>
@@ -1534,7 +1525,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E7" s="5">
         <v>7.4</v>
@@ -1550,7 +1541,7 @@
         <v>512</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8" s="5">
         <v>7.1</v>
@@ -1566,7 +1557,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5">
         <v>7.4</v>
@@ -1582,7 +1573,7 @@
         <v>512</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E10" s="5">
         <v>7</v>
@@ -1598,7 +1589,7 @@
         <v>64</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="5">
         <v>7.2</v>
@@ -1614,7 +1605,7 @@
         <v>512</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" s="5">
         <v>6.9</v>
@@ -1630,7 +1621,7 @@
         <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5">
         <v>7.4</v>
@@ -1646,7 +1637,7 @@
         <v>512</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14" s="5">
         <v>7.1</v>
@@ -1662,7 +1653,7 @@
         <v>64</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E15" s="4">
         <v>7.6</v>
@@ -1688,59 +1679,59 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F5"/>
+      <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="A1" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="43"/>
-      <c r="C2" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="28"/>
+      <c r="A2" s="44"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="30" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="30"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="46"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="E3" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" s="34" t="s">
-        <v>69</v>
+      <c r="A3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="5">
@@ -1751,10 +1742,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="5">
@@ -1779,58 +1770,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tables: fix SCF baseline, add w2v dim 1024
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\docs\2023_interspeech_features\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A2A1CE-DF0B-4E06-81CC-61BECCB5BE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D4098A-84F0-4B97-A129-609B0B7E7434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t>Effect of pre-training the wav2vec 2.0 feature extractor using the unsupervised loss on the same data (LibriSpeech 960h).</t>
+  </si>
+  <si>
+    <t>26k</t>
+  </si>
+  <si>
+    <t>15.5M</t>
   </si>
 </sst>
 </file>
@@ -262,11 +268,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -512,17 +525,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -531,25 +544,25 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -561,36 +574,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -821,12 +837,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -842,7 +858,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="32"/>
@@ -856,7 +872,7 @@
       </c>
       <c r="H2" s="30"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>32</v>
       </c>
@@ -882,7 +898,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -902,7 +918,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>49</v>
       </c>
@@ -918,7 +934,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -928,17 +944,17 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>24</v>
+      <c r="D6" s="48" t="s">
+        <v>72</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
-        <v>7.1</v>
+        <v>7</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -978,9 +994,9 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
@@ -992,7 +1008,7 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="30" t="s">
@@ -1004,7 +1020,7 @@
       </c>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>33</v>
       </c>
@@ -1024,7 +1040,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1038,7 +1054,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1052,7 +1068,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1085,12 +1101,12 @@
       <selection activeCell="E2" sqref="E2:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.453125" style="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
         <v>30</v>
       </c>
@@ -1102,7 +1118,7 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="31"/>
       <c r="C2" s="30" t="s">
@@ -1114,7 +1130,7 @@
       </c>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="20" t="s">
         <v>60</v>
       </c>
@@ -1134,7 +1150,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>64</v>
       </c>
@@ -1147,7 +1163,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>128</v>
       </c>
@@ -1160,7 +1176,7 @@
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>160</v>
       </c>
@@ -1173,7 +1189,7 @@
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>256</v>
       </c>
@@ -1186,7 +1202,7 @@
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>400</v>
       </c>
@@ -1215,15 +1231,15 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="11.453125" style="1"/>
+    <col min="5" max="5" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>56</v>
       </c>
@@ -1241,7 +1257,7 @@
       <c r="G1" s="40"/>
       <c r="H1" s="40"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>57</v>
       </c>
@@ -1259,7 +1275,7 @@
       </c>
       <c r="H2" s="40"/>
     </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="17" t="s">
         <v>58</v>
@@ -1283,7 +1299,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35">
         <v>5</v>
       </c>
@@ -1303,7 +1319,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
       <c r="B5" s="10">
         <v>150</v>
@@ -1321,7 +1337,7 @@
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
       <c r="B6" s="10">
         <v>200</v>
@@ -1339,7 +1355,7 @@
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
       <c r="B7" s="10">
         <v>250</v>
@@ -1357,7 +1373,7 @@
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -1377,7 +1393,7 @@
       <c r="G8" s="11"/>
       <c r="H8" s="11"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
@@ -1410,19 +1426,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>7</v>
       </c>
@@ -1439,7 +1455,7 @@
       <c r="F1" s="30"/>
       <c r="G1" s="30"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="41"/>
       <c r="B2" s="32"/>
       <c r="C2" s="32"/>
@@ -1452,7 +1468,7 @@
       </c>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42"/>
       <c r="B3" s="43"/>
       <c r="C3" s="43"/>
@@ -1469,197 +1485,213 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
-        <v>512</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>1024</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>73</v>
       </c>
       <c r="E4" s="5">
         <v>6.8</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F4" s="46"/>
+      <c r="G4" s="47"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" s="5">
-        <v>7.1</v>
+        <v>6.8</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>128</v>
+        <v>256</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5">
-        <v>7.2</v>
+        <v>7.1</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" s="5">
-        <v>7.4</v>
+        <v>7.2</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="5">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E9" s="5">
-        <v>7.4</v>
+        <v>7.1</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E10" s="5">
-        <v>7</v>
+        <v>7.4</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E11" s="5">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B12">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E12" s="5">
-        <v>6.9</v>
+        <v>7.2</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E13" s="5">
-        <v>7.4</v>
+        <v>6.9</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>512</v>
+        <v>64</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E14" s="5">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15">
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="4">
-        <v>7.6</v>
+        <v>10</v>
+      </c>
+      <c r="E15" s="5">
+        <v>7.1</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4">
+        <v>7.6</v>
+      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1682,9 +1714,9 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="44" t="s">
         <v>45</v>
       </c>
@@ -1698,7 +1730,7 @@
       <c r="E1" s="30"/>
       <c r="F1" s="30"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="44"/>
       <c r="B2" s="32"/>
       <c r="C2" s="30" t="s">
@@ -1710,7 +1742,7 @@
       </c>
       <c r="F2" s="30"/>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="45"/>
       <c r="B3" s="43"/>
       <c r="C3" s="24" t="s">
@@ -1726,7 +1758,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1772,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -1770,13 +1802,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1784,7 +1816,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -1792,7 +1824,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1800,7 +1832,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -1808,7 +1840,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -1816,7 +1848,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
update results for other subsets
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D4098A-84F0-4B97-A129-609B0B7E7434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE29E430-5594-4EA0-AB68-0FA639F9BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -837,7 +837,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,12 +911,16 @@
       <c r="D4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
       <c r="F4" s="1">
         <v>7.1</v>
       </c>
       <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
+      <c r="H4" s="1">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -927,12 +931,18 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>2.9</v>
+      </c>
       <c r="F5" s="4">
         <v>6.9</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="H5" s="1">
+        <v>7.2</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -947,12 +957,16 @@
       <c r="D6" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>2.9</v>
+      </c>
       <c r="F6" s="1">
         <v>7</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="H6" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -967,12 +981,16 @@
       <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>2.9</v>
+      </c>
       <c r="F7" s="1">
         <v>6.8</v>
       </c>
       <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1">
+        <v>7.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -991,7 +1009,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,12 +1065,16 @@
       <c r="B4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>2.9</v>
+      </c>
       <c r="D4" s="1">
         <v>6.8</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1061,12 +1083,16 @@
       <c r="B5" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>2.9</v>
+      </c>
       <c r="D5" s="1">
         <v>6.9</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1075,12 +1101,16 @@
       <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
       <c r="D6" s="1">
         <v>7.1</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>7.8</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1098,7 +1128,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1157,6 +1187,9 @@
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
       <c r="D4" s="1">
         <v>7.2</v>
       </c>
@@ -1170,6 +1203,9 @@
       <c r="B5">
         <v>8</v>
       </c>
+      <c r="C5" s="1">
+        <v>3</v>
+      </c>
       <c r="D5" s="1">
         <v>7.1</v>
       </c>
@@ -1183,11 +1219,16 @@
       <c r="B6">
         <v>10</v>
       </c>
+      <c r="C6" s="1">
+        <v>2.9</v>
+      </c>
       <c r="D6" s="1">
         <v>7</v>
       </c>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1196,11 +1237,16 @@
       <c r="B7">
         <v>16</v>
       </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
       <c r="D7" s="1">
         <v>7.1</v>
       </c>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1208,6 +1254,9 @@
       </c>
       <c r="B8">
         <v>25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2.9</v>
       </c>
       <c r="D8" s="1">
         <v>7.3</v>
@@ -1231,7 +1280,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1312,12 +1361,16 @@
       <c r="D4" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="15">
+        <v>3</v>
+      </c>
       <c r="F4" s="15">
         <v>7.1</v>
       </c>
       <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="H4" s="15">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="35"/>
@@ -1330,12 +1383,16 @@
       <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11">
+        <v>3</v>
+      </c>
       <c r="F5" s="11">
         <v>7.1</v>
       </c>
       <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="H5" s="11">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="35"/>
@@ -1348,7 +1405,9 @@
       <c r="D6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11">
+        <v>2.9</v>
+      </c>
       <c r="F6" s="11">
         <v>7.1</v>
       </c>
@@ -1366,12 +1425,16 @@
       <c r="D7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="11"/>
+      <c r="E7" s="11">
+        <v>3</v>
+      </c>
       <c r="F7" s="11">
         <v>7.3</v>
       </c>
       <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="H7" s="11">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -1386,12 +1449,16 @@
       <c r="D8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="11"/>
+      <c r="E8" s="11">
+        <v>3</v>
+      </c>
       <c r="F8" s="11">
         <v>7.3</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="H8" s="11">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -1404,12 +1471,16 @@
       <c r="D9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="11"/>
+      <c r="E9" s="11">
+        <v>3</v>
+      </c>
       <c r="F9" s="11">
         <v>7.1</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="H9" s="11">
+        <v>7.7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1429,7 +1500,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1495,11 +1566,16 @@
       <c r="C4" s="48" t="s">
         <v>73</v>
       </c>
+      <c r="D4" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E4" s="5">
         <v>6.8</v>
       </c>
       <c r="F4" s="46"/>
-      <c r="G4" s="47"/>
+      <c r="G4" s="47">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1511,11 +1587,16 @@
       <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
+      <c r="D5" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E5" s="5">
         <v>6.8</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>7.5</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1527,11 +1608,16 @@
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="D6" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E6" s="5">
         <v>7.1</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1543,11 +1629,16 @@
       <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
       <c r="E7" s="5">
         <v>7.2</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1559,11 +1650,16 @@
       <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="D8" s="1">
+        <v>3.1</v>
+      </c>
       <c r="E8" s="5">
         <v>7.4</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1575,6 +1671,9 @@
       <c r="C9" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D9" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E9" s="5">
         <v>7.1</v>
       </c>
@@ -1591,11 +1690,16 @@
       <c r="C10" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="D10" s="1">
+        <v>3</v>
+      </c>
       <c r="E10" s="5">
         <v>7.4</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1607,11 +1711,16 @@
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="D11" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E11" s="5">
         <v>7</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="G11" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1623,6 +1732,9 @@
       <c r="C12" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="D12" s="1">
+        <v>3.1</v>
+      </c>
       <c r="E12" s="5">
         <v>7.2</v>
       </c>
@@ -1639,11 +1751,16 @@
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D13" s="1">
+        <v>2.9</v>
+      </c>
       <c r="E13" s="5">
         <v>6.9</v>
       </c>
       <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="G13" s="1">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1655,11 +1772,16 @@
       <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
+      <c r="D14" s="1">
+        <v>3.1</v>
+      </c>
       <c r="E14" s="5">
         <v>7.4</v>
       </c>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1">
+        <v>7.9</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1671,11 +1793,16 @@
       <c r="C15" s="3" t="s">
         <v>10</v>
       </c>
+      <c r="D15" s="1">
+        <v>3</v>
+      </c>
       <c r="E15" s="5">
         <v>7.1</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1">
+        <v>7.7</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1686,6 +1813,9 @@
       </c>
       <c r="C16" s="3" t="s">
         <v>18</v>
+      </c>
+      <c r="D16" s="1">
+        <v>3.1</v>
       </c>
       <c r="E16" s="4">
         <v>7.6</v>
@@ -1711,7 +1841,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:D2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1765,7 +1895,9 @@
       <c r="B4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>2.9</v>
+      </c>
       <c r="D4" s="5">
         <v>7</v>
       </c>
@@ -1779,12 +1911,16 @@
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>2.9</v>
+      </c>
       <c r="D5" s="5">
         <v>6.8</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>7.5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
add more results to tables
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE29E430-5594-4EA0-AB68-0FA639F9BEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A08D2-4195-426A-A0CF-E876F7FBD1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +917,9 @@
       <c r="F4" s="1">
         <v>7.1</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>3.4</v>
+      </c>
       <c r="H4" s="1">
         <v>7.7</v>
       </c>
@@ -987,7 +989,9 @@
       <c r="F7" s="1">
         <v>6.8</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>3.3</v>
+      </c>
       <c r="H7" s="1">
         <v>7.5</v>
       </c>
@@ -1009,7 +1013,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1071,7 +1075,9 @@
       <c r="D4" s="1">
         <v>6.8</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>3.3</v>
+      </c>
       <c r="F4" s="1">
         <v>7.5</v>
       </c>
@@ -1089,7 +1095,9 @@
       <c r="D5" s="1">
         <v>6.9</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>3.3</v>
+      </c>
       <c r="F5" s="1">
         <v>7.5</v>
       </c>
@@ -1107,7 +1115,9 @@
       <c r="D6" s="1">
         <v>7.1</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>3.3</v>
+      </c>
       <c r="F6" s="1">
         <v>7.8</v>
       </c>
@@ -1128,7 +1138,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1204,9 @@
         <v>7.2</v>
       </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1209,8 +1221,12 @@
       <c r="D5" s="1">
         <v>7.1</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F5" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1262,7 +1278,9 @@
         <v>7.3</v>
       </c>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>7.7</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1280,7 +1298,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,7 +1407,9 @@
       <c r="F5" s="11">
         <v>7.1</v>
       </c>
-      <c r="G5" s="11"/>
+      <c r="G5" s="11">
+        <v>3.4</v>
+      </c>
       <c r="H5" s="11">
         <v>7.7</v>
       </c>
@@ -1412,7 +1432,9 @@
         <v>7.1</v>
       </c>
       <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="H6" s="11">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="34"/>
@@ -1477,7 +1499,9 @@
       <c r="F9" s="11">
         <v>7.1</v>
       </c>
-      <c r="G9" s="11"/>
+      <c r="G9" s="11">
+        <v>3.4</v>
+      </c>
       <c r="H9" s="11">
         <v>7.7</v>
       </c>
@@ -1499,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1596,9 @@
       <c r="E4" s="5">
         <v>6.8</v>
       </c>
-      <c r="F4" s="46"/>
+      <c r="F4" s="46">
+        <v>3.3</v>
+      </c>
       <c r="G4" s="47">
         <v>7.5</v>
       </c>
@@ -1593,7 +1619,9 @@
       <c r="E5" s="5">
         <v>6.8</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>3.3</v>
+      </c>
       <c r="G5" s="1">
         <v>7.5</v>
       </c>
@@ -1614,7 +1642,9 @@
       <c r="E6" s="5">
         <v>7.1</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>3.4</v>
+      </c>
       <c r="G6" s="1">
         <v>7.6</v>
       </c>
@@ -1656,9 +1686,11 @@
       <c r="E8" s="5">
         <v>7.4</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>3.5</v>
+      </c>
       <c r="G8" s="1">
-        <v>7.6</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1677,7 +1709,9 @@
       <c r="E9" s="5">
         <v>7.1</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>3.4</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1696,7 +1730,9 @@
       <c r="E10" s="5">
         <v>7.4</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>3.5</v>
+      </c>
       <c r="G10" s="1">
         <v>7.9</v>
       </c>
@@ -1717,7 +1753,9 @@
       <c r="E11" s="5">
         <v>7</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>3.3</v>
+      </c>
       <c r="G11" s="1">
         <v>7.6</v>
       </c>
@@ -1738,8 +1776,12 @@
       <c r="E12" s="5">
         <v>7.2</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="G12" s="1">
+        <v>7.8</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1757,7 +1799,9 @@
       <c r="E13" s="5">
         <v>6.9</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1">
+        <v>3.3</v>
+      </c>
       <c r="G13" s="1">
         <v>7.4</v>
       </c>
@@ -1778,7 +1822,9 @@
       <c r="E14" s="5">
         <v>7.4</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1">
+        <v>3.5</v>
+      </c>
       <c r="G14" s="1">
         <v>7.9</v>
       </c>
@@ -1799,7 +1845,9 @@
       <c r="E15" s="5">
         <v>7.1</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1">
+        <v>3.5</v>
+      </c>
       <c r="G15" s="1">
         <v>7.7</v>
       </c>
@@ -1820,8 +1868,12 @@
       <c r="E16" s="4">
         <v>7.6</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="G16" s="1">
+        <v>8.1999999999999993</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1841,7 +1893,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1901,8 +1953,12 @@
       <c r="D4" s="5">
         <v>7</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="E4" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>7.4</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1917,7 +1973,9 @@
       <c r="D5" s="5">
         <v>6.8</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="1">
+        <v>3.4</v>
+      </c>
       <c r="F5" s="1">
         <v>7.5</v>
       </c>

</xml_diff>

<commit_message>
add remaining missing numbers
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6A08D2-4195-426A-A0CF-E876F7FBD1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B81F3-22D6-4AF4-93AC-FBC31C6777CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -837,7 +837,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +965,9 @@
       <c r="F6" s="1">
         <v>7</v>
       </c>
-      <c r="G6" s="1"/>
+      <c r="G6" s="1">
+        <v>3.4</v>
+      </c>
       <c r="H6" s="1">
         <v>7.6</v>
       </c>
@@ -1138,7 +1140,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1203,7 +1205,9 @@
       <c r="D4" s="1">
         <v>7.2</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="1">
+        <v>3.4</v>
+      </c>
       <c r="F4" s="1">
         <v>7.8</v>
       </c>
@@ -1241,7 +1245,9 @@
       <c r="D6" s="1">
         <v>7</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="1">
+        <v>3.4</v>
+      </c>
       <c r="F6" s="1">
         <v>7.6</v>
       </c>
@@ -1259,7 +1265,9 @@
       <c r="D7" s="1">
         <v>7.1</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="1">
+        <v>3.4</v>
+      </c>
       <c r="F7" s="1">
         <v>7.7</v>
       </c>
@@ -1277,7 +1285,9 @@
       <c r="D8" s="1">
         <v>7.3</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="1">
+        <v>3.4</v>
+      </c>
       <c r="F8" s="1">
         <v>7.7</v>
       </c>
@@ -1298,7 +1308,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,7 +1395,9 @@
       <c r="F4" s="15">
         <v>7.1</v>
       </c>
-      <c r="G4" s="15"/>
+      <c r="G4" s="15">
+        <v>3.3</v>
+      </c>
       <c r="H4" s="15">
         <v>7.8</v>
       </c>
@@ -1431,7 +1443,9 @@
       <c r="F6" s="11">
         <v>7.1</v>
       </c>
-      <c r="G6" s="11"/>
+      <c r="G6" s="11">
+        <v>3.4</v>
+      </c>
       <c r="H6" s="11">
         <v>7.8</v>
       </c>
@@ -1453,7 +1467,9 @@
       <c r="F7" s="11">
         <v>7.3</v>
       </c>
-      <c r="G7" s="11"/>
+      <c r="G7" s="11">
+        <v>3.4</v>
+      </c>
       <c r="H7" s="11">
         <v>7.8</v>
       </c>
@@ -1477,7 +1493,9 @@
       <c r="F8" s="11">
         <v>7.3</v>
       </c>
-      <c r="G8" s="11"/>
+      <c r="G8" s="11">
+        <v>3.4</v>
+      </c>
       <c r="H8" s="11">
         <v>7.7</v>
       </c>
@@ -1524,7 +1542,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1665,7 +1683,9 @@
       <c r="E7" s="5">
         <v>7.2</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>3.4</v>
+      </c>
       <c r="G7" s="1">
         <v>7.7</v>
       </c>
@@ -1712,7 +1732,9 @@
       <c r="F9" s="1">
         <v>3.4</v>
       </c>
-      <c r="G9" s="1"/>
+      <c r="G9" s="1">
+        <v>7.6</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">

</xml_diff>

<commit_message>
update text, add increasing w2v dims
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64B81F3-22D6-4AF4-93AC-FBC31C6777CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00813F0A-EE58-45FB-870C-2E9E8BC12ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -259,6 +259,21 @@
   </si>
   <si>
     <t>15.5M</t>
+  </si>
+  <si>
+    <t>64-512</t>
+  </si>
+  <si>
+    <t>128-1024</t>
+  </si>
+  <si>
+    <t>3.3M</t>
+  </si>
+  <si>
+    <t>5.0M</t>
+  </si>
+  <si>
+    <t>1.0M</t>
   </si>
 </sst>
 </file>
@@ -525,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -607,6 +622,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -836,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1156,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1539,10 +1555,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,6 +1911,63 @@
       </c>
       <c r="G16" s="1">
         <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D18" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="E18" s="49">
+        <v>7</v>
+      </c>
+      <c r="F18" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="G18" s="1">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D19" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="E19" s="49">
+        <v>6.9</v>
+      </c>
+      <c r="F19" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="G19" s="1">
+        <v>7.4</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +2091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
small text updates, mel params in table 1
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Documents\text\2023_interspeech_features\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\peter\i6\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00813F0A-EE58-45FB-870C-2E9E8BC12ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBE2172-EDCD-4A5D-94D5-3AA6ECFA909E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28890" windowHeight="16740" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35085" yWindow="3105" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -274,6 +274,12 @@
   </si>
   <si>
     <t>1.0M</t>
+  </si>
+  <si>
+    <t>21k</t>
+  </si>
+  <si>
+    <t>74.2M</t>
   </si>
 </sst>
 </file>
@@ -283,11 +289,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -540,17 +553,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -559,25 +572,29 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -589,40 +606,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -852,43 +866,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="32" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="32"/>
-      <c r="E1" s="30" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="30" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="34"/>
+      <c r="G2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="30"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="34"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
         <v>32</v>
       </c>
@@ -914,7 +928,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>49</v>
       </c>
@@ -940,15 +954,19 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>49</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>79</v>
+      </c>
       <c r="E5" s="1">
         <v>2.9</v>
       </c>
@@ -962,7 +980,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -972,7 +990,7 @@
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="32" t="s">
         <v>72</v>
       </c>
       <c r="E6" s="1">
@@ -988,7 +1006,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1034,33 +1052,33 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="30" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="23" t="s">
         <v>33</v>
       </c>
@@ -1080,7 +1098,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1100,7 +1118,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>23</v>
       </c>
@@ -1120,7 +1138,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>22</v>
       </c>
@@ -1159,36 +1177,36 @@
       <selection activeCell="F6" sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="30" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
         <v>60</v>
       </c>
@@ -1208,7 +1226,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>64</v>
       </c>
@@ -1228,7 +1246,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>128</v>
       </c>
@@ -1248,7 +1266,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>160</v>
       </c>
@@ -1268,7 +1286,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>256</v>
       </c>
@@ -1288,7 +1306,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>400</v>
       </c>
@@ -1327,48 +1345,48 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="11.42578125" style="1"/>
+    <col min="5" max="5" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>56</v>
       </c>
       <c r="B1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="37"/>
-      <c r="E1" s="40" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
         <v>57</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="40" t="s">
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40" t="s">
+      <c r="F2" s="44"/>
+      <c r="G2" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="40"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16"/>
       <c r="B3" s="17" t="s">
         <v>58</v>
@@ -1392,8 +1410,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+    <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="39">
         <v>5</v>
       </c>
       <c r="B4" s="12">
@@ -1418,8 +1436,8 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="35"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
       <c r="B5" s="10">
         <v>150</v>
       </c>
@@ -1442,8 +1460,8 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="35"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="39"/>
       <c r="B6" s="10">
         <v>200</v>
       </c>
@@ -1466,8 +1484,8 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="34"/>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="38"/>
       <c r="B7" s="10">
         <v>250</v>
       </c>
@@ -1490,11 +1508,11 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="37">
         <v>150</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1516,11 +1534,11 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="38"/>
       <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
@@ -1561,46 +1579,46 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="41"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="30" t="s">
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="45"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30" t="s">
+      <c r="E2" s="34"/>
+      <c r="F2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="30"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="42"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
+      <c r="G2" s="34"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47"/>
+      <c r="C3" s="47"/>
       <c r="D3" s="24" t="s">
         <v>63</v>
       </c>
@@ -1614,14 +1632,14 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>6</v>
       </c>
       <c r="B4">
         <v>1024</v>
       </c>
-      <c r="C4" s="48" t="s">
+      <c r="C4" s="32" t="s">
         <v>73</v>
       </c>
       <c r="D4" s="1">
@@ -1630,14 +1648,14 @@
       <c r="E4" s="5">
         <v>6.8</v>
       </c>
-      <c r="F4" s="46">
+      <c r="F4" s="30">
         <v>3.3</v>
       </c>
-      <c r="G4" s="47">
+      <c r="G4" s="31">
         <v>7.5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
@@ -1660,7 +1678,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>6</v>
       </c>
@@ -1683,7 +1701,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1706,7 +1724,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1729,7 +1747,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1752,7 +1770,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1775,7 +1793,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1798,7 +1816,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1821,7 +1839,7 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3</v>
       </c>
@@ -1844,7 +1862,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3</v>
       </c>
@@ -1867,7 +1885,7 @@
         <v>7.9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1890,7 +1908,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1913,18 +1931,18 @@
         <v>8.1999999999999993</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>6</v>
       </c>
       <c r="B17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="32" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1937,7 +1955,7 @@
       <c r="D18" s="1">
         <v>2.9</v>
       </c>
-      <c r="E18" s="49">
+      <c r="E18" s="33">
         <v>7</v>
       </c>
       <c r="F18" s="1">
@@ -1947,7 +1965,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1960,7 +1978,7 @@
       <c r="D19" s="1">
         <v>2.9</v>
       </c>
-      <c r="E19" s="49">
+      <c r="E19" s="33">
         <v>6.9</v>
       </c>
       <c r="F19" s="1">
@@ -1991,37 +2009,37 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="30" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="48"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="D2" s="34"/>
+      <c r="E2" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="30"/>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="43"/>
+      <c r="F2" s="34"/>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="49"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="24" t="s">
         <v>63</v>
       </c>
@@ -2035,7 +2053,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -2055,7 +2073,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
@@ -2091,13 +2109,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2105,7 +2123,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -2113,7 +2131,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2121,7 +2139,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -2137,7 +2155,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
add results: w2v dim 64-515, scf masking
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\peter\i6\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBE2172-EDCD-4A5D-94D5-3AA6ECFA909E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BB8B127-4747-4C6F-8C8B-86AAB2FEAEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35085" yWindow="3105" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33915" yWindow="3015" windowWidth="14445" windowHeight="9765" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
     <sheet name="pretraining" sheetId="11" r:id="rId2"/>
     <sheet name="window_size" sheetId="9" r:id="rId3"/>
     <sheet name="scf_size" sheetId="10" r:id="rId4"/>
-    <sheet name="w2v_size" sheetId="6" r:id="rId5"/>
-    <sheet name="w2v_proj" sheetId="12" r:id="rId6"/>
-    <sheet name="_Caption" sheetId="5" r:id="rId7"/>
+    <sheet name="scf_mask" sheetId="13" r:id="rId5"/>
+    <sheet name="w2v_size" sheetId="6" r:id="rId6"/>
+    <sheet name="w2v_proj" sheetId="12" r:id="rId7"/>
+    <sheet name="_Caption" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
   <si>
     <t>Feature Extractor</t>
   </si>
@@ -280,6 +281,12 @@
   </si>
   <si>
     <t>74.2M</t>
+  </si>
+  <si>
+    <t>#Masked Filters</t>
+  </si>
+  <si>
+    <t>WER</t>
   </si>
 </sst>
 </file>
@@ -289,11 +296,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -553,17 +567,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -572,29 +586,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -606,37 +621,37 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -866,41 +881,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE527AF-55A2-41AA-8F14-181B057D8090}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="34" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="34" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34" t="s">
+      <c r="F2" s="35"/>
+      <c r="G2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="34"/>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
@@ -961,10 +976,10 @@
       <c r="B5" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D5" s="34" t="s">
         <v>79</v>
       </c>
       <c r="E5" s="1">
@@ -1055,28 +1070,28 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="34" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="23" t="s">
@@ -1183,28 +1198,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="34" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="34" t="s">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="20" t="s">
@@ -1357,16 +1372,16 @@
       <c r="B1" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="41"/>
-      <c r="E1" s="44" t="s">
+      <c r="D1" s="42"/>
+      <c r="E1" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="26" t="s">
@@ -1375,16 +1390,16 @@
       <c r="B2" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44" t="s">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44" t="s">
+      <c r="F2" s="45"/>
+      <c r="G2" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="16"/>
@@ -1411,7 +1426,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="39">
+      <c r="A4" s="40">
         <v>5</v>
       </c>
       <c r="B4" s="12">
@@ -1437,7 +1452,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
+      <c r="A5" s="40"/>
       <c r="B5" s="10">
         <v>150</v>
       </c>
@@ -1461,7 +1476,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="39"/>
+      <c r="A6" s="40"/>
       <c r="B6" s="10">
         <v>200</v>
       </c>
@@ -1485,7 +1500,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="38"/>
+      <c r="A7" s="39"/>
       <c r="B7" s="10">
         <v>250</v>
       </c>
@@ -1512,7 +1527,7 @@
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="37">
+      <c r="B8" s="38">
         <v>150</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1538,7 +1553,7 @@
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="38"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="10" t="s">
         <v>44</v>
       </c>
@@ -1572,11 +1587,138 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06808640-2533-4C1B-86A0-7CC207E6508A}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>30</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>40</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>80</v>
+      </c>
+      <c r="B14" s="1">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1586,39 +1728,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="45"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="34" t="s">
+      <c r="A2" s="46"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="34"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="46"/>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
+      <c r="A3" s="47"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
       <c r="D3" s="24" t="s">
         <v>63</v>
       </c>
@@ -1940,6 +2082,18 @@
       </c>
       <c r="C17" s="32" t="s">
         <v>78</v>
+      </c>
+      <c r="D17" s="1">
+        <v>3</v>
+      </c>
+      <c r="E17" s="51">
+        <v>7.1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="G17" s="1">
+        <v>7.7</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2001,7 +2155,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A375FB06-3221-44DD-B2E3-EEAFC4F977A3}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -2012,34 +2166,34 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="48"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="34" t="s">
+      <c r="A2" s="49"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="F2" s="34"/>
+      <c r="F2" s="35"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="49"/>
-      <c r="B3" s="47"/>
+      <c r="A3" s="50"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="24" t="s">
         <v>63</v>
       </c>
@@ -2105,7 +2259,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>

</xml_diff>

<commit_message>
fix w2v dim 64-512 numbers (now epoch 490)
</commit_message>
<xml_diff>
--- a/tables/features.xlsx
+++ b/tables/features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\peter\i6\Documents\text\2023_interspeech_features\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FF77D4-BD0B-416A-ABDE-AA1AFD686A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2230E4-6919-4B92-B50B-358278EE8467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="8" r:id="rId1"/>
@@ -1718,8 +1718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793B9E34-3081-4C73-80A5-9A4848EE5D6D}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2091,10 +2091,10 @@
         <v>7.1</v>
       </c>
       <c r="F17" s="1">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="G17" s="1">
-        <v>7.7</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
@@ -2264,7 +2264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>